<commit_message>
Updated Leave Card 1/26/2024 4:34 pm
</commit_message>
<xml_diff>
--- a/REGULAR/DIMARANAN, REYNALDO.xlsx
+++ b/REGULAR/DIMARANAN, REYNALDO.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\dole-pc\Users\DOLE\Desktop\LEAVE-CARD\REGULAR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DOLE\Desktop\LEAVE-CARD\REGULAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784F6CB5-CC72-490B-BEA3-C8CEB805B343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="2018 LEAVE CREDITS" sheetId="1" r:id="rId1"/>
@@ -27,7 +26,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'2017 LEAVE BALANCE'!$1:$9</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'2018 LEAVE CREDITS'!$1:$9</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -624,7 +623,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
@@ -1540,7 +1539,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -1557,25 +1556,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A8:K392" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:K392" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="PERIOD" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="PARTICULARS" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="EARNED" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Absence Undertime W/ Pay" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="BALANCE" dataDxfId="21">
+    <tableColumn id="1" name="PERIOD" dataDxfId="25"/>
+    <tableColumn id="2" name="PARTICULARS" dataDxfId="24"/>
+    <tableColumn id="3" name="EARNED" dataDxfId="23"/>
+    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="22"/>
+    <tableColumn id="5" name="BALANCE" dataDxfId="21">
       <calculatedColumnFormula>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Absence Undertime W/O Pay" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="EARNED " dataDxfId="19">
+    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="20"/>
+    <tableColumn id="7" name="EARNED " dataDxfId="19">
       <calculatedColumnFormula>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Absence Undertime  W/ Pay" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="BALANCE " dataDxfId="17">
+    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="18"/>
+    <tableColumn id="9" name="BALANCE " dataDxfId="17">
       <calculatedColumnFormula>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Absence Undertime  W/O Pay" dataDxfId="16"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="REMARKS" dataDxfId="15"/>
+    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="16"/>
+    <tableColumn id="11" name="REMARKS" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1587,25 +1586,25 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A8:K59" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A8:K59" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="PERIOD" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="PARTICULARS" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="EARNED" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Absence Undertime W/ Pay" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="BALANCE" dataDxfId="6">
+    <tableColumn id="1" name="PERIOD" dataDxfId="10"/>
+    <tableColumn id="2" name="PARTICULARS" dataDxfId="9"/>
+    <tableColumn id="3" name="EARNED" dataDxfId="8"/>
+    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="7"/>
+    <tableColumn id="5" name="BALANCE" dataDxfId="6">
       <calculatedColumnFormula>SUM(Table13[EARNED])-SUM(Table13[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Absence Undertime W/O Pay" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="EARNED " dataDxfId="4">
+    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="5"/>
+    <tableColumn id="7" name="EARNED " dataDxfId="4">
       <calculatedColumnFormula>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Absence Undertime  W/ Pay" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="BALANCE " dataDxfId="2">
+    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="3"/>
+    <tableColumn id="9" name="BALANCE " dataDxfId="2">
       <calculatedColumnFormula>SUM(Table13[[EARNED ]])-SUM(Table13[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Absence Undertime  W/O Pay" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="REMARKS" dataDxfId="0"/>
+    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="1"/>
+    <tableColumn id="11" name="REMARKS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1912,34 +1911,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:K392"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2304" topLeftCell="A334" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2310" topLeftCell="A334" activePane="bottomLeft"/>
       <selection activeCell="I9" sqref="I9"/>
-      <selection pane="bottomLeft" activeCell="D351" sqref="D351"/>
+      <selection pane="bottomLeft" activeCell="F351" sqref="F351"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
@@ -1960,7 +1959,7 @@
       <c r="J2" s="54"/>
       <c r="K2" s="55"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
@@ -1982,7 +1981,7 @@
       <c r="J3" s="56"/>
       <c r="K3" s="57"/>
     </row>
-    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
@@ -2004,7 +2003,7 @@
       <c r="J4" s="54"/>
       <c r="K4" s="55"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="H5" s="27" t="s">
         <v>18</v>
@@ -2012,7 +2011,7 @@
       <c r="I5" s="27"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31"/>
@@ -2025,7 +2024,7 @@
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="C7" s="52" t="s">
@@ -2042,7 +2041,7 @@
       <c r="J7" s="52"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -2077,7 +2076,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>23</v>
@@ -2086,7 +2085,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="13">
         <f>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])</f>
-        <v>140.05500000000006</v>
+        <v>141.30500000000006</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="13" t="str">
@@ -2096,12 +2095,12 @@
       <c r="H9" s="11"/>
       <c r="I9" s="13">
         <f>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])</f>
-        <v>169.16700000000003</v>
+        <v>170.41700000000003</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="48" t="s">
         <v>73</v>
       </c>
@@ -2123,7 +2122,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="23">
         <v>37928</v>
       </c>
@@ -2149,7 +2148,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="23"/>
       <c r="B12" s="20" t="s">
         <v>54</v>
@@ -2171,7 +2170,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="23"/>
       <c r="B13" s="20" t="s">
         <v>80</v>
@@ -2191,7 +2190,7 @@
       <c r="J13" s="11"/>
       <c r="K13" s="20"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="23">
         <v>37956</v>
       </c>
@@ -2215,7 +2214,7 @@
       <c r="J14" s="11"/>
       <c r="K14" s="20"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="48" t="s">
         <v>79</v>
       </c>
@@ -2233,7 +2232,7 @@
       <c r="J15" s="11"/>
       <c r="K15" s="20"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="23">
         <v>37987</v>
       </c>
@@ -2259,7 +2258,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="23"/>
       <c r="B17" s="20" t="s">
         <v>84</v>
@@ -2278,7 +2277,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="23"/>
       <c r="B18" s="20" t="s">
         <v>85</v>
@@ -2295,7 +2294,7 @@
       <c r="J18" s="11"/>
       <c r="K18" s="20"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="23">
         <v>38018</v>
       </c>
@@ -2317,7 +2316,7 @@
       <c r="J19" s="11"/>
       <c r="K19" s="20"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="23"/>
       <c r="B20" s="20" t="s">
         <v>86</v>
@@ -2338,7 +2337,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="23">
         <v>38047</v>
       </c>
@@ -2362,7 +2361,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="40"/>
       <c r="B22" s="20" t="s">
         <v>88</v>
@@ -2382,7 +2381,7 @@
       <c r="J22" s="11"/>
       <c r="K22" s="20"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="23">
         <v>38078</v>
       </c>
@@ -2408,7 +2407,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
       <c r="B24" s="20" t="s">
         <v>89</v>
@@ -2428,7 +2427,7 @@
       <c r="J24" s="11"/>
       <c r="K24" s="20"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="23">
         <v>38108</v>
       </c>
@@ -2454,7 +2453,7 @@
         <v>38121</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="23"/>
       <c r="B26" s="20" t="s">
         <v>49</v>
@@ -2473,7 +2472,7 @@
         <v>38119</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="23"/>
       <c r="B27" s="20" t="s">
         <v>54</v>
@@ -2492,7 +2491,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="23"/>
       <c r="B28" s="20" t="s">
         <v>93</v>
@@ -2509,7 +2508,7 @@
       <c r="J28" s="11"/>
       <c r="K28" s="20"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="23">
         <v>38139</v>
       </c>
@@ -2535,7 +2534,7 @@
         <v>38160</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="23">
         <v>38169</v>
       </c>
@@ -2561,7 +2560,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="23"/>
       <c r="B31" s="20" t="s">
         <v>49</v>
@@ -2583,7 +2582,7 @@
         <v>38191</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="23"/>
       <c r="B32" s="20" t="s">
         <v>49</v>
@@ -2605,7 +2604,7 @@
         <v>38198</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="23"/>
       <c r="B33" s="20" t="s">
         <v>96</v>
@@ -2625,7 +2624,7 @@
       <c r="J33" s="11"/>
       <c r="K33" s="49"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="23">
         <v>38200</v>
       </c>
@@ -2651,7 +2650,7 @@
         <v>38225</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="23"/>
       <c r="B35" s="20" t="s">
         <v>97</v>
@@ -2671,7 +2670,7 @@
       <c r="J35" s="11"/>
       <c r="K35" s="49"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="23">
         <v>38231</v>
       </c>
@@ -2697,7 +2696,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="23"/>
       <c r="B37" s="20" t="s">
         <v>98</v>
@@ -2717,7 +2716,7 @@
       <c r="J37" s="11"/>
       <c r="K37" s="20"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="23">
         <v>38261</v>
       </c>
@@ -2743,7 +2742,7 @@
         <v>38264</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="23"/>
       <c r="B39" s="20" t="s">
         <v>100</v>
@@ -2760,7 +2759,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="23"/>
       <c r="B40" s="20" t="s">
         <v>54</v>
@@ -2779,7 +2778,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="23">
         <v>38292</v>
       </c>
@@ -2805,7 +2804,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="23"/>
       <c r="B42" s="20" t="s">
         <v>54</v>
@@ -2827,7 +2826,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="23">
         <v>38322</v>
       </c>
@@ -2847,7 +2846,7 @@
       <c r="J43" s="11"/>
       <c r="K43" s="20"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="48" t="s">
         <v>105</v>
       </c>
@@ -2865,7 +2864,7 @@
       <c r="J44" s="11"/>
       <c r="K44" s="20"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="23">
         <v>38353</v>
       </c>
@@ -2889,7 +2888,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="23"/>
       <c r="B46" s="20" t="s">
         <v>107</v>
@@ -2911,7 +2910,7 @@
         <v>38387</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="23">
         <v>38384</v>
       </c>
@@ -2935,7 +2934,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="20"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="23">
         <v>38412</v>
       </c>
@@ -2961,7 +2960,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="23"/>
       <c r="B49" s="20" t="s">
         <v>54</v>
@@ -2980,7 +2979,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="23"/>
       <c r="B50" s="20" t="s">
         <v>54</v>
@@ -2999,7 +2998,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="23"/>
       <c r="B51" s="20" t="s">
         <v>110</v>
@@ -3016,7 +3015,7 @@
       <c r="J51" s="11"/>
       <c r="K51" s="20"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="23">
         <v>38443</v>
       </c>
@@ -3040,7 +3039,7 @@
       <c r="J52" s="11"/>
       <c r="K52" s="20"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="23">
         <v>38473</v>
       </c>
@@ -3066,7 +3065,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="23"/>
       <c r="B54" s="20" t="s">
         <v>107</v>
@@ -3085,7 +3084,7 @@
         <v>38496</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="23"/>
       <c r="B55" s="20" t="s">
         <v>115</v>
@@ -3102,7 +3101,7 @@
       <c r="J55" s="11"/>
       <c r="K55" s="20"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="23">
         <v>38504</v>
       </c>
@@ -3128,7 +3127,7 @@
         <v>38518</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="23"/>
       <c r="B57" s="20" t="s">
         <v>49</v>
@@ -3147,7 +3146,7 @@
         <v>38523</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="23"/>
       <c r="B58" s="20" t="s">
         <v>117</v>
@@ -3164,7 +3163,7 @@
       <c r="J58" s="11"/>
       <c r="K58" s="20"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="23">
         <v>38534</v>
       </c>
@@ -3190,7 +3189,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="23"/>
       <c r="B60" s="20" t="s">
         <v>54</v>
@@ -3209,7 +3208,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="23"/>
       <c r="B61" s="20" t="s">
         <v>118</v>
@@ -3226,7 +3225,7 @@
       <c r="J61" s="11"/>
       <c r="K61" s="20"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="23">
         <v>38565</v>
       </c>
@@ -3252,7 +3251,7 @@
         <v>38569</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="23"/>
       <c r="B63" s="20" t="s">
         <v>50</v>
@@ -3271,7 +3270,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="23"/>
       <c r="B64" s="20" t="s">
         <v>50</v>
@@ -3290,7 +3289,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="23"/>
       <c r="B65" s="20" t="s">
         <v>121</v>
@@ -3307,7 +3306,7 @@
       <c r="J65" s="11"/>
       <c r="K65" s="20"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="23">
         <v>38596</v>
       </c>
@@ -3333,7 +3332,7 @@
         <v>38607</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="23"/>
       <c r="B67" s="20" t="s">
         <v>122</v>
@@ -3350,7 +3349,7 @@
       <c r="J67" s="11"/>
       <c r="K67" s="20"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="23">
         <v>38626</v>
       </c>
@@ -3376,7 +3375,7 @@
         <v>38639</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="23"/>
       <c r="B69" s="20" t="s">
         <v>49</v>
@@ -3395,7 +3394,7 @@
         <v>38644</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="23"/>
       <c r="B70" s="20" t="s">
         <v>49</v>
@@ -3414,7 +3413,7 @@
         <v>38654</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="23"/>
       <c r="B71" s="20" t="s">
         <v>123</v>
@@ -3431,7 +3430,7 @@
       <c r="J71" s="11"/>
       <c r="K71" s="20"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="23">
         <v>38657</v>
       </c>
@@ -3457,7 +3456,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="23"/>
       <c r="B73" s="20" t="s">
         <v>49</v>
@@ -3476,7 +3475,7 @@
         <v>38667</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="23"/>
       <c r="B74" s="20" t="s">
         <v>49</v>
@@ -3495,7 +3494,7 @@
         <v>38674</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="23"/>
       <c r="B75" s="20" t="s">
         <v>49</v>
@@ -3514,7 +3513,7 @@
         <v>38679</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="23"/>
       <c r="B76" s="20" t="s">
         <v>126</v>
@@ -3531,7 +3530,7 @@
       <c r="J76" s="11"/>
       <c r="K76" s="20"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="23">
         <v>38687</v>
       </c>
@@ -3555,7 +3554,7 @@
       <c r="J77" s="11"/>
       <c r="K77" s="20"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="48" t="s">
         <v>129</v>
       </c>
@@ -3570,7 +3569,7 @@
       <c r="J78" s="11"/>
       <c r="K78" s="20"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="23">
         <v>38718</v>
       </c>
@@ -3594,7 +3593,7 @@
       <c r="J79" s="11"/>
       <c r="K79" s="20"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="23">
         <v>38749</v>
       </c>
@@ -3620,7 +3619,7 @@
         <v>38765</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="23"/>
       <c r="B81" s="20" t="s">
         <v>49</v>
@@ -3639,7 +3638,7 @@
         <v>38773</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="23"/>
       <c r="B82" s="20" t="s">
         <v>131</v>
@@ -3659,7 +3658,7 @@
       <c r="J82" s="11"/>
       <c r="K82" s="49"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="23">
         <v>38777</v>
       </c>
@@ -3683,7 +3682,7 @@
       <c r="J83" s="11"/>
       <c r="K83" s="20"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="23">
         <v>38808</v>
       </c>
@@ -3709,7 +3708,7 @@
         <v>38825</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="23"/>
       <c r="B85" s="20" t="s">
         <v>50</v>
@@ -3728,7 +3727,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="23"/>
       <c r="B86" s="20" t="s">
         <v>91</v>
@@ -3745,7 +3744,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="23"/>
       <c r="B87" s="20" t="s">
         <v>91</v>
@@ -3762,7 +3761,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="23"/>
       <c r="B88" s="20" t="s">
         <v>133</v>
@@ -3779,7 +3778,7 @@
       <c r="J88" s="11"/>
       <c r="K88" s="20"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="23">
         <v>38838</v>
       </c>
@@ -3803,7 +3802,7 @@
       <c r="J89" s="11"/>
       <c r="K89" s="20"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="23">
         <v>38869</v>
       </c>
@@ -3827,7 +3826,7 @@
       <c r="J90" s="11"/>
       <c r="K90" s="20"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="23">
         <v>38899</v>
       </c>
@@ -3853,7 +3852,7 @@
         <v>38908</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="23"/>
       <c r="B92" s="20" t="s">
         <v>50</v>
@@ -3872,7 +3871,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="23"/>
       <c r="B93" s="20" t="s">
         <v>139</v>
@@ -3889,7 +3888,7 @@
       <c r="J93" s="11"/>
       <c r="K93" s="20"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="23">
         <v>38930</v>
       </c>
@@ -3915,7 +3914,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="23"/>
       <c r="B95" s="20" t="s">
         <v>143</v>
@@ -3932,7 +3931,7 @@
       <c r="J95" s="11"/>
       <c r="K95" s="20"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="23">
         <v>38961</v>
       </c>
@@ -3958,7 +3957,7 @@
         <v>38968</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="23"/>
       <c r="B97" s="20" t="s">
         <v>141</v>
@@ -3978,7 +3977,7 @@
       <c r="J97" s="11"/>
       <c r="K97" s="20"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="23">
         <v>38991</v>
       </c>
@@ -4004,7 +4003,7 @@
         <v>39010</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="23"/>
       <c r="B99" s="20" t="s">
         <v>49</v>
@@ -4023,7 +4022,7 @@
         <v>39023</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="23"/>
       <c r="B100" s="20" t="s">
         <v>144</v>
@@ -4040,7 +4039,7 @@
       <c r="J100" s="11"/>
       <c r="K100" s="20"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="23">
         <v>39022</v>
       </c>
@@ -4066,7 +4065,7 @@
         <v>39034</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="23"/>
       <c r="B102" s="20" t="s">
         <v>145</v>
@@ -4086,7 +4085,7 @@
       <c r="J102" s="11"/>
       <c r="K102" s="20"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="23">
         <v>39052</v>
       </c>
@@ -4112,7 +4111,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="23"/>
       <c r="B104" s="20" t="s">
         <v>56</v>
@@ -4129,7 +4128,7 @@
       <c r="J104" s="11"/>
       <c r="K104" s="20"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="23"/>
       <c r="B105" s="20" t="s">
         <v>147</v>
@@ -4146,7 +4145,7 @@
       <c r="J105" s="11"/>
       <c r="K105" s="20"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="48" t="s">
         <v>148</v>
       </c>
@@ -4164,7 +4163,7 @@
       <c r="J106" s="11"/>
       <c r="K106" s="20"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="23">
         <v>39083</v>
       </c>
@@ -4188,7 +4187,7 @@
       <c r="J107" s="11"/>
       <c r="K107" s="20"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="23">
         <v>39114</v>
       </c>
@@ -4214,7 +4213,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="23"/>
       <c r="B109" s="20" t="s">
         <v>49</v>
@@ -4233,7 +4232,7 @@
         <v>39132</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="23"/>
       <c r="B110" s="20" t="s">
         <v>54</v>
@@ -4252,7 +4251,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="23"/>
       <c r="B111" s="20" t="s">
         <v>151</v>
@@ -4269,7 +4268,7 @@
       <c r="J111" s="11"/>
       <c r="K111" s="20"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="23">
         <v>39142</v>
       </c>
@@ -4295,7 +4294,7 @@
         <v>39146</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="23"/>
       <c r="B113" s="20" t="s">
         <v>49</v>
@@ -4314,7 +4313,7 @@
         <v>39155</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="23"/>
       <c r="B114" s="20" t="s">
         <v>154</v>
@@ -4331,7 +4330,7 @@
       <c r="J114" s="11"/>
       <c r="K114" s="20"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="23">
         <v>39173</v>
       </c>
@@ -4357,7 +4356,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="23"/>
       <c r="B116" s="20" t="s">
         <v>49</v>
@@ -4376,7 +4375,7 @@
         <v>39199</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="23">
         <v>39203</v>
       </c>
@@ -4402,7 +4401,7 @@
         <v>39211</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="23"/>
       <c r="B118" s="20" t="s">
         <v>156</v>
@@ -4421,7 +4420,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="23"/>
       <c r="B119" s="20" t="s">
         <v>157</v>
@@ -4438,7 +4437,7 @@
       <c r="J119" s="11"/>
       <c r="K119" s="20"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="23">
         <v>39234</v>
       </c>
@@ -4464,7 +4463,7 @@
         <v>39262</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="23">
         <v>39264</v>
       </c>
@@ -4490,7 +4489,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="23">
         <v>39295</v>
       </c>
@@ -4510,7 +4509,7 @@
       <c r="J122" s="11"/>
       <c r="K122" s="20"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="23">
         <v>39326</v>
       </c>
@@ -4530,7 +4529,7 @@
       <c r="J123" s="11"/>
       <c r="K123" s="20"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="23">
         <v>39356</v>
       </c>
@@ -4550,7 +4549,7 @@
       <c r="J124" s="11"/>
       <c r="K124" s="20"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="23">
         <v>39387</v>
       </c>
@@ -4570,7 +4569,7 @@
       <c r="J125" s="11"/>
       <c r="K125" s="20"/>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="23">
         <v>39417</v>
       </c>
@@ -4594,7 +4593,7 @@
       <c r="J126" s="11"/>
       <c r="K126" s="20"/>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="48" t="s">
         <v>149</v>
       </c>
@@ -4612,7 +4611,7 @@
       <c r="J127" s="11"/>
       <c r="K127" s="20"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="23">
         <v>39448</v>
       </c>
@@ -4632,7 +4631,7 @@
       <c r="J128" s="11"/>
       <c r="K128" s="20"/>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="23">
         <v>39479</v>
       </c>
@@ -4652,7 +4651,7 @@
       <c r="J129" s="11"/>
       <c r="K129" s="20"/>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="23">
         <v>39508</v>
       </c>
@@ -4672,7 +4671,7 @@
       <c r="J130" s="11"/>
       <c r="K130" s="20"/>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="23">
         <v>39539</v>
       </c>
@@ -4692,7 +4691,7 @@
       <c r="J131" s="11"/>
       <c r="K131" s="20"/>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="23">
         <v>39569</v>
       </c>
@@ -4712,7 +4711,7 @@
       <c r="J132" s="11"/>
       <c r="K132" s="20"/>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="23">
         <v>39600</v>
       </c>
@@ -4732,7 +4731,7 @@
       <c r="J133" s="11"/>
       <c r="K133" s="20"/>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="23">
         <v>39630</v>
       </c>
@@ -4752,7 +4751,7 @@
       <c r="J134" s="11"/>
       <c r="K134" s="20"/>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="23">
         <v>39661</v>
       </c>
@@ -4772,7 +4771,7 @@
       <c r="J135" s="11"/>
       <c r="K135" s="20"/>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="23">
         <v>39692</v>
       </c>
@@ -4792,7 +4791,7 @@
       <c r="J136" s="11"/>
       <c r="K136" s="20"/>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="23">
         <v>39722</v>
       </c>
@@ -4812,7 +4811,7 @@
       <c r="J137" s="11"/>
       <c r="K137" s="20"/>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="23">
         <v>39753</v>
       </c>
@@ -4832,7 +4831,7 @@
       <c r="J138" s="11"/>
       <c r="K138" s="20"/>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="23">
         <v>39783</v>
       </c>
@@ -4856,7 +4855,7 @@
       <c r="J139" s="11"/>
       <c r="K139" s="20"/>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" s="48" t="s">
         <v>160</v>
       </c>
@@ -4871,7 +4870,7 @@
       <c r="J140" s="11"/>
       <c r="K140" s="20"/>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" s="23">
         <v>39814</v>
       </c>
@@ -4891,7 +4890,7 @@
       <c r="J141" s="11"/>
       <c r="K141" s="20"/>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" s="23">
         <v>39845</v>
       </c>
@@ -4911,7 +4910,7 @@
       <c r="J142" s="11"/>
       <c r="K142" s="20"/>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" s="23">
         <v>39873</v>
       </c>
@@ -4931,7 +4930,7 @@
       <c r="J143" s="11"/>
       <c r="K143" s="20"/>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" s="23">
         <v>39904</v>
       </c>
@@ -4951,7 +4950,7 @@
       <c r="J144" s="11"/>
       <c r="K144" s="20"/>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" s="23">
         <v>39934</v>
       </c>
@@ -4971,7 +4970,7 @@
       <c r="J145" s="11"/>
       <c r="K145" s="20"/>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" s="23">
         <v>39965</v>
       </c>
@@ -4991,7 +4990,7 @@
       <c r="J146" s="11"/>
       <c r="K146" s="20"/>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" s="23">
         <v>39995</v>
       </c>
@@ -5011,7 +5010,7 @@
       <c r="J147" s="11"/>
       <c r="K147" s="20"/>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" s="23">
         <v>40026</v>
       </c>
@@ -5031,7 +5030,7 @@
       <c r="J148" s="11"/>
       <c r="K148" s="20"/>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" s="23">
         <v>40057</v>
       </c>
@@ -5051,7 +5050,7 @@
       <c r="J149" s="11"/>
       <c r="K149" s="20"/>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" s="23">
         <v>40087</v>
       </c>
@@ -5071,7 +5070,7 @@
       <c r="J150" s="11"/>
       <c r="K150" s="20"/>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" s="23">
         <v>40118</v>
       </c>
@@ -5091,7 +5090,7 @@
       <c r="J151" s="11"/>
       <c r="K151" s="20"/>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" s="23">
         <v>40148</v>
       </c>
@@ -5115,7 +5114,7 @@
       <c r="J152" s="11"/>
       <c r="K152" s="20"/>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" s="48" t="s">
         <v>162</v>
       </c>
@@ -5130,7 +5129,7 @@
       <c r="J153" s="11"/>
       <c r="K153" s="20"/>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="23">
         <v>40179</v>
       </c>
@@ -5150,7 +5149,7 @@
       <c r="J154" s="11"/>
       <c r="K154" s="20"/>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" s="23">
         <v>40210</v>
       </c>
@@ -5170,7 +5169,7 @@
       <c r="J155" s="11"/>
       <c r="K155" s="20"/>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" s="23">
         <v>40238</v>
       </c>
@@ -5190,7 +5189,7 @@
       <c r="J156" s="11"/>
       <c r="K156" s="20"/>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" s="23">
         <v>40269</v>
       </c>
@@ -5210,7 +5209,7 @@
       <c r="J157" s="11"/>
       <c r="K157" s="20"/>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" s="23">
         <v>40299</v>
       </c>
@@ -5230,7 +5229,7 @@
       <c r="J158" s="11"/>
       <c r="K158" s="20"/>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" s="23">
         <v>40330</v>
       </c>
@@ -5250,7 +5249,7 @@
       <c r="J159" s="11"/>
       <c r="K159" s="20"/>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" s="23">
         <v>40360</v>
       </c>
@@ -5270,7 +5269,7 @@
       <c r="J160" s="11"/>
       <c r="K160" s="20"/>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" s="23">
         <v>40391</v>
       </c>
@@ -5290,7 +5289,7 @@
       <c r="J161" s="11"/>
       <c r="K161" s="20"/>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" s="23">
         <v>40422</v>
       </c>
@@ -5310,7 +5309,7 @@
       <c r="J162" s="11"/>
       <c r="K162" s="20"/>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" s="23">
         <v>40452</v>
       </c>
@@ -5330,7 +5329,7 @@
       <c r="J163" s="11"/>
       <c r="K163" s="20"/>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="23">
         <v>40483</v>
       </c>
@@ -5350,7 +5349,7 @@
       <c r="J164" s="11"/>
       <c r="K164" s="20"/>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" s="23">
         <v>40513</v>
       </c>
@@ -5374,7 +5373,7 @@
       <c r="J165" s="11"/>
       <c r="K165" s="20"/>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" s="48" t="s">
         <v>163</v>
       </c>
@@ -5392,7 +5391,7 @@
       <c r="J166" s="11"/>
       <c r="K166" s="20"/>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" s="23">
         <v>40544</v>
       </c>
@@ -5412,7 +5411,7 @@
       <c r="J167" s="11"/>
       <c r="K167" s="20"/>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" s="23">
         <v>40575</v>
       </c>
@@ -5432,7 +5431,7 @@
       <c r="J168" s="11"/>
       <c r="K168" s="20"/>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" s="23">
         <v>40603</v>
       </c>
@@ -5452,7 +5451,7 @@
       <c r="J169" s="11"/>
       <c r="K169" s="20"/>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" s="23">
         <v>40634</v>
       </c>
@@ -5472,7 +5471,7 @@
       <c r="J170" s="11"/>
       <c r="K170" s="20"/>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" s="23">
         <v>40664</v>
       </c>
@@ -5492,7 +5491,7 @@
       <c r="J171" s="11"/>
       <c r="K171" s="20"/>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" s="23">
         <v>40695</v>
       </c>
@@ -5512,7 +5511,7 @@
       <c r="J172" s="11"/>
       <c r="K172" s="20"/>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" s="23">
         <v>40725</v>
       </c>
@@ -5532,7 +5531,7 @@
       <c r="J173" s="11"/>
       <c r="K173" s="20"/>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" s="23">
         <v>40756</v>
       </c>
@@ -5552,7 +5551,7 @@
       <c r="J174" s="11"/>
       <c r="K174" s="20"/>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" s="23">
         <v>40787</v>
       </c>
@@ -5572,7 +5571,7 @@
       <c r="J175" s="11"/>
       <c r="K175" s="20"/>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" s="23">
         <v>40817</v>
       </c>
@@ -5592,7 +5591,7 @@
       <c r="J176" s="11"/>
       <c r="K176" s="20"/>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" s="23">
         <v>40848</v>
       </c>
@@ -5612,7 +5611,7 @@
       <c r="J177" s="11"/>
       <c r="K177" s="20"/>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" s="23">
         <v>40878</v>
       </c>
@@ -5638,7 +5637,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179" s="23"/>
       <c r="B179" s="20" t="s">
         <v>91</v>
@@ -5655,7 +5654,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" s="23"/>
       <c r="B180" s="20" t="s">
         <v>161</v>
@@ -5672,7 +5671,7 @@
       <c r="J180" s="11"/>
       <c r="K180" s="20"/>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181" s="48" t="s">
         <v>166</v>
       </c>
@@ -5687,7 +5686,7 @@
       <c r="J181" s="11"/>
       <c r="K181" s="20"/>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" s="23">
         <v>40909</v>
       </c>
@@ -5707,7 +5706,7 @@
       <c r="J182" s="11"/>
       <c r="K182" s="20"/>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" s="23">
         <v>40940</v>
       </c>
@@ -5727,7 +5726,7 @@
       <c r="J183" s="11"/>
       <c r="K183" s="20"/>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" s="23">
         <v>40969</v>
       </c>
@@ -5753,7 +5752,7 @@
         <v>40614</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" s="23">
         <v>41000</v>
       </c>
@@ -5773,7 +5772,7 @@
       <c r="J185" s="11"/>
       <c r="K185" s="20"/>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" s="23">
         <v>41030</v>
       </c>
@@ -5793,7 +5792,7 @@
       <c r="J186" s="11"/>
       <c r="K186" s="20"/>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" s="23">
         <v>41061</v>
       </c>
@@ -5813,7 +5812,7 @@
       <c r="J187" s="11"/>
       <c r="K187" s="20"/>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" s="23">
         <v>41091</v>
       </c>
@@ -5833,7 +5832,7 @@
       <c r="J188" s="11"/>
       <c r="K188" s="20"/>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" s="23">
         <v>41122</v>
       </c>
@@ -5853,7 +5852,7 @@
       <c r="J189" s="11"/>
       <c r="K189" s="20"/>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" s="23">
         <v>41153</v>
       </c>
@@ -5873,7 +5872,7 @@
       <c r="J190" s="11"/>
       <c r="K190" s="20"/>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" s="23">
         <v>41183</v>
       </c>
@@ -5893,7 +5892,7 @@
       <c r="J191" s="11"/>
       <c r="K191" s="20"/>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192" s="23">
         <v>41214</v>
       </c>
@@ -5917,7 +5916,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193" s="23"/>
       <c r="B193" s="20" t="s">
         <v>56</v>
@@ -5939,7 +5938,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194" s="23">
         <v>41244</v>
       </c>
@@ -5959,7 +5958,7 @@
       <c r="J194" s="11"/>
       <c r="K194" s="20"/>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195" s="48" t="s">
         <v>169</v>
       </c>
@@ -5977,7 +5976,7 @@
       <c r="J195" s="11"/>
       <c r="K195" s="20"/>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196" s="23">
         <v>41275</v>
       </c>
@@ -5997,7 +5996,7 @@
       <c r="J196" s="11"/>
       <c r="K196" s="20"/>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197" s="23">
         <v>41306</v>
       </c>
@@ -6017,7 +6016,7 @@
       <c r="J197" s="11"/>
       <c r="K197" s="20"/>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198" s="23">
         <v>41334</v>
       </c>
@@ -6037,7 +6036,7 @@
       <c r="J198" s="11"/>
       <c r="K198" s="20"/>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199" s="23">
         <v>41365</v>
       </c>
@@ -6057,7 +6056,7 @@
       <c r="J199" s="11"/>
       <c r="K199" s="20"/>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200" s="23">
         <v>41395</v>
       </c>
@@ -6077,7 +6076,7 @@
       <c r="J200" s="11"/>
       <c r="K200" s="20"/>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A201" s="23">
         <v>41426</v>
       </c>
@@ -6097,7 +6096,7 @@
       <c r="J201" s="11"/>
       <c r="K201" s="20"/>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A202" s="23">
         <v>41456</v>
       </c>
@@ -6117,7 +6116,7 @@
       <c r="J202" s="11"/>
       <c r="K202" s="20"/>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A203" s="23">
         <v>41487</v>
       </c>
@@ -6137,7 +6136,7 @@
       <c r="J203" s="11"/>
       <c r="K203" s="20"/>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A204" s="23">
         <v>41518</v>
       </c>
@@ -6157,7 +6156,7 @@
       <c r="J204" s="11"/>
       <c r="K204" s="20"/>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A205" s="23">
         <v>41548</v>
       </c>
@@ -6177,7 +6176,7 @@
       <c r="J205" s="11"/>
       <c r="K205" s="20"/>
     </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A206" s="23">
         <v>41579</v>
       </c>
@@ -6201,7 +6200,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A207" s="23"/>
       <c r="B207" s="20" t="s">
         <v>56</v>
@@ -6220,7 +6219,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A208" s="23">
         <v>41609</v>
       </c>
@@ -6240,7 +6239,7 @@
       <c r="J208" s="11"/>
       <c r="K208" s="20"/>
     </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A209" s="48" t="s">
         <v>172</v>
       </c>
@@ -6258,7 +6257,7 @@
       <c r="J209" s="11"/>
       <c r="K209" s="20"/>
     </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A210" s="23">
         <v>41640</v>
       </c>
@@ -6278,7 +6277,7 @@
       <c r="J210" s="11"/>
       <c r="K210" s="20"/>
     </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A211" s="23">
         <v>41671</v>
       </c>
@@ -6298,7 +6297,7 @@
       <c r="J211" s="11"/>
       <c r="K211" s="20"/>
     </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A212" s="23">
         <v>41699</v>
       </c>
@@ -6324,7 +6323,7 @@
         <v>41724</v>
       </c>
     </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A213" s="23"/>
       <c r="B213" s="20" t="s">
         <v>173</v>
@@ -6344,7 +6343,7 @@
       <c r="J213" s="11"/>
       <c r="K213" s="20"/>
     </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214" s="23">
         <v>41730</v>
       </c>
@@ -6364,7 +6363,7 @@
       <c r="J214" s="11"/>
       <c r="K214" s="20"/>
     </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A215" s="23">
         <v>41760</v>
       </c>
@@ -6388,7 +6387,7 @@
       <c r="J215" s="11"/>
       <c r="K215" s="20"/>
     </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A216" s="23">
         <v>41791</v>
       </c>
@@ -6412,7 +6411,7 @@
       <c r="J216" s="11"/>
       <c r="K216" s="20"/>
     </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A217" s="23">
         <v>41821</v>
       </c>
@@ -6436,7 +6435,7 @@
       <c r="J217" s="11"/>
       <c r="K217" s="20"/>
     </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A218" s="23">
         <v>41852</v>
       </c>
@@ -6460,7 +6459,7 @@
       <c r="J218" s="11"/>
       <c r="K218" s="20"/>
     </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A219" s="23">
         <v>41883</v>
       </c>
@@ -6480,7 +6479,7 @@
       <c r="J219" s="11"/>
       <c r="K219" s="20"/>
     </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A220" s="23">
         <v>41913</v>
       </c>
@@ -6504,7 +6503,7 @@
       <c r="J220" s="11"/>
       <c r="K220" s="20"/>
     </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A221" s="23">
         <v>41944</v>
       </c>
@@ -6530,7 +6529,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A222" s="23">
         <v>41974</v>
       </c>
@@ -6554,7 +6553,7 @@
       <c r="J222" s="11"/>
       <c r="K222" s="20"/>
     </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A223" s="48" t="s">
         <v>178</v>
       </c>
@@ -6572,7 +6571,7 @@
       <c r="J223" s="11"/>
       <c r="K223" s="20"/>
     </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A224" s="23">
         <v>42005</v>
       </c>
@@ -6596,7 +6595,7 @@
       <c r="J224" s="11"/>
       <c r="K224" s="20"/>
     </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A225" s="23">
         <v>42036</v>
       </c>
@@ -6616,7 +6615,7 @@
       <c r="J225" s="11"/>
       <c r="K225" s="20"/>
     </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A226" s="23">
         <v>42064</v>
       </c>
@@ -6636,7 +6635,7 @@
       <c r="J226" s="11"/>
       <c r="K226" s="20"/>
     </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A227" s="23">
         <v>42095</v>
       </c>
@@ -6656,7 +6655,7 @@
       <c r="J227" s="11"/>
       <c r="K227" s="20"/>
     </row>
-    <row r="228" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A228" s="23">
         <v>42125</v>
       </c>
@@ -6676,7 +6675,7 @@
       <c r="J228" s="11"/>
       <c r="K228" s="20"/>
     </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A229" s="23">
         <v>42156</v>
       </c>
@@ -6696,7 +6695,7 @@
       <c r="J229" s="11"/>
       <c r="K229" s="20"/>
     </row>
-    <row r="230" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A230" s="23">
         <v>42186</v>
       </c>
@@ -6720,7 +6719,7 @@
       <c r="J230" s="11"/>
       <c r="K230" s="20"/>
     </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A231" s="23">
         <v>42217</v>
       </c>
@@ -6740,7 +6739,7 @@
       <c r="J231" s="11"/>
       <c r="K231" s="20"/>
     </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A232" s="23">
         <v>42248</v>
       </c>
@@ -6760,7 +6759,7 @@
       <c r="J232" s="11"/>
       <c r="K232" s="20"/>
     </row>
-    <row r="233" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A233" s="23">
         <v>42278</v>
       </c>
@@ -6780,7 +6779,7 @@
       <c r="J233" s="11"/>
       <c r="K233" s="20"/>
     </row>
-    <row r="234" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A234" s="23">
         <v>42309</v>
       </c>
@@ -6800,7 +6799,7 @@
       <c r="J234" s="11"/>
       <c r="K234" s="20"/>
     </row>
-    <row r="235" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A235" s="23">
         <v>42339</v>
       </c>
@@ -6824,7 +6823,7 @@
       <c r="J235" s="11"/>
       <c r="K235" s="20"/>
     </row>
-    <row r="236" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A236" s="23"/>
       <c r="B236" s="20" t="s">
         <v>181</v>
@@ -6844,7 +6843,7 @@
       <c r="J236" s="11"/>
       <c r="K236" s="20"/>
     </row>
-    <row r="237" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A237" s="48" t="s">
         <v>182</v>
       </c>
@@ -6862,7 +6861,7 @@
       <c r="J237" s="11"/>
       <c r="K237" s="20"/>
     </row>
-    <row r="238" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A238" s="23">
         <v>42370</v>
       </c>
@@ -6882,7 +6881,7 @@
       <c r="J238" s="11"/>
       <c r="K238" s="20"/>
     </row>
-    <row r="239" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A239" s="23">
         <v>42401</v>
       </c>
@@ -6902,7 +6901,7 @@
       <c r="J239" s="11"/>
       <c r="K239" s="20"/>
     </row>
-    <row r="240" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A240" s="23">
         <v>42430</v>
       </c>
@@ -6922,7 +6921,7 @@
       <c r="J240" s="11"/>
       <c r="K240" s="20"/>
     </row>
-    <row r="241" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A241" s="23">
         <v>42461</v>
       </c>
@@ -6942,7 +6941,7 @@
       <c r="J241" s="11"/>
       <c r="K241" s="20"/>
     </row>
-    <row r="242" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A242" s="23">
         <v>42491</v>
       </c>
@@ -6962,7 +6961,7 @@
       <c r="J242" s="11"/>
       <c r="K242" s="20"/>
     </row>
-    <row r="243" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A243" s="23">
         <v>42522</v>
       </c>
@@ -6982,7 +6981,7 @@
       <c r="J243" s="11"/>
       <c r="K243" s="20"/>
     </row>
-    <row r="244" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A244" s="23">
         <v>42552</v>
       </c>
@@ -7002,7 +7001,7 @@
       <c r="J244" s="11"/>
       <c r="K244" s="20"/>
     </row>
-    <row r="245" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A245" s="23">
         <v>42583</v>
       </c>
@@ -7028,7 +7027,7 @@
         <v>42633</v>
       </c>
     </row>
-    <row r="246" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A246" s="23"/>
       <c r="B246" s="20" t="s">
         <v>49</v>
@@ -7048,7 +7047,7 @@
       <c r="J246" s="11"/>
       <c r="K246" s="20"/>
     </row>
-    <row r="247" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A247" s="23">
         <v>42614</v>
       </c>
@@ -7068,7 +7067,7 @@
       <c r="J247" s="11"/>
       <c r="K247" s="20"/>
     </row>
-    <row r="248" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A248" s="23">
         <v>42644</v>
       </c>
@@ -7094,7 +7093,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="249" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A249" s="23"/>
       <c r="B249" s="20" t="s">
         <v>49</v>
@@ -7116,7 +7115,7 @@
         <v>42682</v>
       </c>
     </row>
-    <row r="250" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A250" s="23">
         <v>42675</v>
       </c>
@@ -7142,7 +7141,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="251" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A251" s="23">
         <v>42705</v>
       </c>
@@ -7166,7 +7165,7 @@
       <c r="J251" s="11"/>
       <c r="K251" s="20"/>
     </row>
-    <row r="252" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A252" s="48" t="s">
         <v>185</v>
       </c>
@@ -7184,7 +7183,7 @@
       <c r="J252" s="11"/>
       <c r="K252" s="20"/>
     </row>
-    <row r="253" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A253" s="23">
         <v>42736</v>
       </c>
@@ -7208,7 +7207,7 @@
       <c r="J253" s="11"/>
       <c r="K253" s="20"/>
     </row>
-    <row r="254" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A254" s="23">
         <v>42767</v>
       </c>
@@ -7234,7 +7233,7 @@
         <v>42791</v>
       </c>
     </row>
-    <row r="255" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A255" s="23"/>
       <c r="B255" s="20" t="s">
         <v>187</v>
@@ -7254,7 +7253,7 @@
       <c r="J255" s="11"/>
       <c r="K255" s="20"/>
     </row>
-    <row r="256" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A256" s="23">
         <v>42795</v>
       </c>
@@ -7280,7 +7279,7 @@
         <v>42822</v>
       </c>
     </row>
-    <row r="257" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A257" s="23"/>
       <c r="B257" s="20" t="s">
         <v>188</v>
@@ -7300,7 +7299,7 @@
       <c r="J257" s="11"/>
       <c r="K257" s="20"/>
     </row>
-    <row r="258" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A258" s="23">
         <v>42826</v>
       </c>
@@ -7320,7 +7319,7 @@
       <c r="J258" s="11"/>
       <c r="K258" s="20"/>
     </row>
-    <row r="259" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A259" s="23">
         <v>42856</v>
       </c>
@@ -7346,7 +7345,7 @@
         <v>42858</v>
       </c>
     </row>
-    <row r="260" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A260" s="23"/>
       <c r="B260" s="20" t="s">
         <v>49</v>
@@ -7365,7 +7364,7 @@
         <v>42865</v>
       </c>
     </row>
-    <row r="261" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A261" s="23">
         <v>42887</v>
       </c>
@@ -7391,7 +7390,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="262" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A262" s="23">
         <v>42917</v>
       </c>
@@ -7411,7 +7410,7 @@
       <c r="J262" s="11"/>
       <c r="K262" s="20"/>
     </row>
-    <row r="263" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A263" s="23">
         <v>42948</v>
       </c>
@@ -7437,7 +7436,7 @@
         <v>43026</v>
       </c>
     </row>
-    <row r="264" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A264" s="23">
         <v>42979</v>
       </c>
@@ -7457,7 +7456,7 @@
       <c r="J264" s="11"/>
       <c r="K264" s="20"/>
     </row>
-    <row r="265" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A265" s="23">
         <v>43009</v>
       </c>
@@ -7477,7 +7476,7 @@
       <c r="J265" s="11"/>
       <c r="K265" s="20"/>
     </row>
-    <row r="266" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A266" s="23">
         <v>43040</v>
       </c>
@@ -7497,7 +7496,7 @@
       <c r="J266" s="11"/>
       <c r="K266" s="20"/>
     </row>
-    <row r="267" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A267" s="23">
         <v>43070</v>
       </c>
@@ -7521,7 +7520,7 @@
       <c r="J267" s="11"/>
       <c r="K267" s="20"/>
     </row>
-    <row r="268" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A268" s="48" t="s">
         <v>44</v>
       </c>
@@ -7539,7 +7538,7 @@
       <c r="J268" s="11"/>
       <c r="K268" s="20"/>
     </row>
-    <row r="269" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A269" s="40">
         <v>43101</v>
       </c>
@@ -7565,7 +7564,7 @@
         <v>43131</v>
       </c>
     </row>
-    <row r="270" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A270" s="40">
         <v>43132</v>
       </c>
@@ -7585,7 +7584,7 @@
       <c r="J270" s="11"/>
       <c r="K270" s="20"/>
     </row>
-    <row r="271" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A271" s="40">
         <v>43160</v>
       </c>
@@ -7605,7 +7604,7 @@
       <c r="J271" s="11"/>
       <c r="K271" s="20"/>
     </row>
-    <row r="272" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A272" s="40">
         <v>43191</v>
       </c>
@@ -7625,7 +7624,7 @@
       <c r="J272" s="11"/>
       <c r="K272" s="20"/>
     </row>
-    <row r="273" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A273" s="40">
         <v>43221</v>
       </c>
@@ -7651,7 +7650,7 @@
         <v>43217</v>
       </c>
     </row>
-    <row r="274" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A274" s="40"/>
       <c r="B274" s="20" t="s">
         <v>50</v>
@@ -7670,7 +7669,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="275" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A275" s="40">
         <v>43252</v>
       </c>
@@ -7690,7 +7689,7 @@
       <c r="J275" s="12"/>
       <c r="K275" s="15"/>
     </row>
-    <row r="276" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A276" s="40">
         <v>43282</v>
       </c>
@@ -7710,7 +7709,7 @@
       <c r="J276" s="11"/>
       <c r="K276" s="20"/>
     </row>
-    <row r="277" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A277" s="40">
         <v>43313</v>
       </c>
@@ -7736,7 +7735,7 @@
         <v>43319</v>
       </c>
     </row>
-    <row r="278" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A278" s="40">
         <v>43344</v>
       </c>
@@ -7756,7 +7755,7 @@
       <c r="J278" s="11"/>
       <c r="K278" s="20"/>
     </row>
-    <row r="279" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A279" s="40">
         <v>43374</v>
       </c>
@@ -7776,7 +7775,7 @@
       <c r="J279" s="11"/>
       <c r="K279" s="20"/>
     </row>
-    <row r="280" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A280" s="40">
         <v>43405</v>
       </c>
@@ -7796,7 +7795,7 @@
       <c r="J280" s="11"/>
       <c r="K280" s="20"/>
     </row>
-    <row r="281" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A281" s="40">
         <v>43435</v>
       </c>
@@ -7822,7 +7821,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="282" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A282" s="48" t="s">
         <v>45</v>
       </c>
@@ -7840,7 +7839,7 @@
       <c r="J282" s="11"/>
       <c r="K282" s="20"/>
     </row>
-    <row r="283" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A283" s="40">
         <v>43466</v>
       </c>
@@ -7860,7 +7859,7 @@
       <c r="J283" s="11"/>
       <c r="K283" s="20"/>
     </row>
-    <row r="284" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A284" s="40">
         <v>43497</v>
       </c>
@@ -7880,7 +7879,7 @@
       <c r="J284" s="11"/>
       <c r="K284" s="20"/>
     </row>
-    <row r="285" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A285" s="40">
         <v>43525</v>
       </c>
@@ -7900,7 +7899,7 @@
       <c r="J285" s="11"/>
       <c r="K285" s="20"/>
     </row>
-    <row r="286" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A286" s="40">
         <v>43556</v>
       </c>
@@ -7926,7 +7925,7 @@
         <v>43613</v>
       </c>
     </row>
-    <row r="287" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A287" s="40">
         <v>43586</v>
       </c>
@@ -7946,7 +7945,7 @@
       <c r="J287" s="11"/>
       <c r="K287" s="20"/>
     </row>
-    <row r="288" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A288" s="40">
         <v>43617</v>
       </c>
@@ -7966,7 +7965,7 @@
       <c r="J288" s="11"/>
       <c r="K288" s="20"/>
     </row>
-    <row r="289" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A289" s="40">
         <v>43647</v>
       </c>
@@ -7986,7 +7985,7 @@
       <c r="J289" s="11"/>
       <c r="K289" s="20"/>
     </row>
-    <row r="290" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A290" s="40">
         <v>43678</v>
       </c>
@@ -8006,7 +8005,7 @@
       <c r="J290" s="11"/>
       <c r="K290" s="20"/>
     </row>
-    <row r="291" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A291" s="40">
         <v>43709</v>
       </c>
@@ -8032,7 +8031,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="292" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A292" s="40">
         <v>43739</v>
       </c>
@@ -8052,7 +8051,7 @@
       <c r="J292" s="11"/>
       <c r="K292" s="20"/>
     </row>
-    <row r="293" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A293" s="40">
         <v>43770</v>
       </c>
@@ -8078,7 +8077,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="294" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A294" s="40">
         <v>43800</v>
       </c>
@@ -8102,7 +8101,7 @@
       <c r="J294" s="11"/>
       <c r="K294" s="20"/>
     </row>
-    <row r="295" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A295" s="48" t="s">
         <v>46</v>
       </c>
@@ -8120,7 +8119,7 @@
       <c r="J295" s="11"/>
       <c r="K295" s="20"/>
     </row>
-    <row r="296" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A296" s="40">
         <v>43831</v>
       </c>
@@ -8144,7 +8143,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="297" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A297" s="40"/>
       <c r="B297" s="20" t="s">
         <v>54</v>
@@ -8161,7 +8160,7 @@
       <c r="J297" s="11"/>
       <c r="K297" s="20"/>
     </row>
-    <row r="298" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A298" s="40">
         <v>43862</v>
       </c>
@@ -8185,7 +8184,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="299" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A299" s="40">
         <v>43891</v>
       </c>
@@ -8205,7 +8204,7 @@
       <c r="J299" s="11"/>
       <c r="K299" s="20"/>
     </row>
-    <row r="300" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A300" s="40">
         <v>43922</v>
       </c>
@@ -8225,7 +8224,7 @@
       <c r="J300" s="11"/>
       <c r="K300" s="20"/>
     </row>
-    <row r="301" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A301" s="40">
         <v>43952</v>
       </c>
@@ -8245,7 +8244,7 @@
       <c r="J301" s="11"/>
       <c r="K301" s="20"/>
     </row>
-    <row r="302" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A302" s="40">
         <v>43983</v>
       </c>
@@ -8265,7 +8264,7 @@
       <c r="J302" s="11"/>
       <c r="K302" s="20"/>
     </row>
-    <row r="303" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A303" s="40">
         <v>44013</v>
       </c>
@@ -8285,7 +8284,7 @@
       <c r="J303" s="11"/>
       <c r="K303" s="20"/>
     </row>
-    <row r="304" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A304" s="40">
         <v>44044</v>
       </c>
@@ -8305,7 +8304,7 @@
       <c r="J304" s="11"/>
       <c r="K304" s="20"/>
     </row>
-    <row r="305" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A305" s="40">
         <v>44075</v>
       </c>
@@ -8325,7 +8324,7 @@
       <c r="J305" s="11"/>
       <c r="K305" s="20"/>
     </row>
-    <row r="306" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A306" s="40">
         <v>44105</v>
       </c>
@@ -8345,7 +8344,7 @@
       <c r="J306" s="11"/>
       <c r="K306" s="20"/>
     </row>
-    <row r="307" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A307" s="40">
         <v>44136</v>
       </c>
@@ -8365,7 +8364,7 @@
       <c r="J307" s="11"/>
       <c r="K307" s="20"/>
     </row>
-    <row r="308" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A308" s="40">
         <v>44166</v>
       </c>
@@ -8389,7 +8388,7 @@
       <c r="J308" s="11"/>
       <c r="K308" s="20"/>
     </row>
-    <row r="309" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A309" s="48" t="s">
         <v>47</v>
       </c>
@@ -8407,7 +8406,7 @@
       <c r="J309" s="11"/>
       <c r="K309" s="20"/>
     </row>
-    <row r="310" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A310" s="40">
         <v>44197</v>
       </c>
@@ -8427,7 +8426,7 @@
       <c r="J310" s="11"/>
       <c r="K310" s="20"/>
     </row>
-    <row r="311" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A311" s="40">
         <v>44228</v>
       </c>
@@ -8447,7 +8446,7 @@
       <c r="J311" s="11"/>
       <c r="K311" s="20"/>
     </row>
-    <row r="312" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A312" s="40">
         <v>44256</v>
       </c>
@@ -8467,7 +8466,7 @@
       <c r="J312" s="11"/>
       <c r="K312" s="20"/>
     </row>
-    <row r="313" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A313" s="40">
         <v>44287</v>
       </c>
@@ -8487,7 +8486,7 @@
       <c r="J313" s="11"/>
       <c r="K313" s="20"/>
     </row>
-    <row r="314" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A314" s="40">
         <v>44317</v>
       </c>
@@ -8507,7 +8506,7 @@
       <c r="J314" s="11"/>
       <c r="K314" s="20"/>
     </row>
-    <row r="315" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A315" s="40">
         <v>44348</v>
       </c>
@@ -8533,7 +8532,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="316" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A316" s="40">
         <v>44378</v>
       </c>
@@ -8553,7 +8552,7 @@
       <c r="J316" s="11"/>
       <c r="K316" s="20"/>
     </row>
-    <row r="317" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A317" s="40">
         <v>44409</v>
       </c>
@@ -8573,7 +8572,7 @@
       <c r="J317" s="11"/>
       <c r="K317" s="20"/>
     </row>
-    <row r="318" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A318" s="40">
         <v>44440</v>
       </c>
@@ -8593,7 +8592,7 @@
       <c r="J318" s="11"/>
       <c r="K318" s="20"/>
     </row>
-    <row r="319" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A319" s="40">
         <v>44470</v>
       </c>
@@ -8613,7 +8612,7 @@
       <c r="J319" s="11"/>
       <c r="K319" s="20"/>
     </row>
-    <row r="320" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A320" s="40">
         <v>44501</v>
       </c>
@@ -8633,7 +8632,7 @@
       <c r="J320" s="11"/>
       <c r="K320" s="20"/>
     </row>
-    <row r="321" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A321" s="40">
         <v>44531</v>
       </c>
@@ -8657,7 +8656,7 @@
       <c r="J321" s="11"/>
       <c r="K321" s="20"/>
     </row>
-    <row r="322" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A322" s="48" t="s">
         <v>48</v>
       </c>
@@ -8675,7 +8674,7 @@
       <c r="J322" s="11"/>
       <c r="K322" s="20"/>
     </row>
-    <row r="323" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A323" s="40">
         <v>44562</v>
       </c>
@@ -8695,7 +8694,7 @@
       <c r="J323" s="11"/>
       <c r="K323" s="20"/>
     </row>
-    <row r="324" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A324" s="40">
         <v>44593</v>
       </c>
@@ -8715,7 +8714,7 @@
       <c r="J324" s="11"/>
       <c r="K324" s="20"/>
     </row>
-    <row r="325" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A325" s="40">
         <v>44621</v>
       </c>
@@ -8735,7 +8734,7 @@
       <c r="J325" s="11"/>
       <c r="K325" s="20"/>
     </row>
-    <row r="326" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A326" s="40">
         <v>44652</v>
       </c>
@@ -8755,7 +8754,7 @@
       <c r="J326" s="11"/>
       <c r="K326" s="20"/>
     </row>
-    <row r="327" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A327" s="40">
         <v>44682</v>
       </c>
@@ -8775,7 +8774,7 @@
       <c r="J327" s="11"/>
       <c r="K327" s="49"/>
     </row>
-    <row r="328" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A328" s="40">
         <v>44713</v>
       </c>
@@ -8795,7 +8794,7 @@
       <c r="J328" s="11"/>
       <c r="K328" s="20"/>
     </row>
-    <row r="329" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A329" s="40">
         <v>44743</v>
       </c>
@@ -8821,7 +8820,7 @@
       <c r="J329" s="11"/>
       <c r="K329" s="20"/>
     </row>
-    <row r="330" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A330" s="40">
         <v>44774</v>
       </c>
@@ -8841,7 +8840,7 @@
       <c r="J330" s="11"/>
       <c r="K330" s="20"/>
     </row>
-    <row r="331" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A331" s="40">
         <v>44805</v>
       </c>
@@ -8861,7 +8860,7 @@
       <c r="J331" s="11"/>
       <c r="K331" s="49"/>
     </row>
-    <row r="332" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A332" s="40">
         <v>44835</v>
       </c>
@@ -8885,7 +8884,7 @@
       <c r="J332" s="11"/>
       <c r="K332" s="20"/>
     </row>
-    <row r="333" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A333" s="40">
         <v>44866</v>
       </c>
@@ -8905,7 +8904,7 @@
       <c r="J333" s="11"/>
       <c r="K333" s="20"/>
     </row>
-    <row r="334" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A334" s="40">
         <v>44896</v>
       </c>
@@ -8929,7 +8928,7 @@
       <c r="J334" s="11"/>
       <c r="K334" s="49"/>
     </row>
-    <row r="335" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A335" s="48" t="s">
         <v>66</v>
       </c>
@@ -8947,7 +8946,7 @@
       <c r="J335" s="11"/>
       <c r="K335" s="20"/>
     </row>
-    <row r="336" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A336" s="40">
         <v>44927</v>
       </c>
@@ -8967,7 +8966,7 @@
       <c r="J336" s="11"/>
       <c r="K336" s="20"/>
     </row>
-    <row r="337" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A337" s="40">
         <v>44958</v>
       </c>
@@ -8987,7 +8986,7 @@
       <c r="J337" s="11"/>
       <c r="K337" s="20"/>
     </row>
-    <row r="338" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A338" s="40">
         <v>44986</v>
       </c>
@@ -9007,7 +9006,7 @@
       <c r="J338" s="11"/>
       <c r="K338" s="20"/>
     </row>
-    <row r="339" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A339" s="40">
         <v>45017</v>
       </c>
@@ -9027,7 +9026,7 @@
       <c r="J339" s="11"/>
       <c r="K339" s="20"/>
     </row>
-    <row r="340" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A340" s="40">
         <v>45047</v>
       </c>
@@ -9047,7 +9046,7 @@
       <c r="J340" s="11"/>
       <c r="K340" s="20"/>
     </row>
-    <row r="341" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A341" s="40">
         <v>45078</v>
       </c>
@@ -9067,7 +9066,7 @@
       <c r="J341" s="11"/>
       <c r="K341" s="20"/>
     </row>
-    <row r="342" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A342" s="40">
         <v>45108</v>
       </c>
@@ -9087,7 +9086,7 @@
       <c r="J342" s="11"/>
       <c r="K342" s="20"/>
     </row>
-    <row r="343" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A343" s="40">
         <v>45139</v>
       </c>
@@ -9107,7 +9106,7 @@
       <c r="J343" s="11"/>
       <c r="K343" s="20"/>
     </row>
-    <row r="344" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A344" s="40">
         <v>45170</v>
       </c>
@@ -9127,7 +9126,7 @@
       <c r="J344" s="11"/>
       <c r="K344" s="20"/>
     </row>
-    <row r="345" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A345" s="40">
         <v>45200</v>
       </c>
@@ -9147,7 +9146,7 @@
       <c r="J345" s="11"/>
       <c r="K345" s="20"/>
     </row>
-    <row r="346" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A346" s="40">
         <v>45231</v>
       </c>
@@ -9167,25 +9166,27 @@
       <c r="J346" s="11"/>
       <c r="K346" s="20"/>
     </row>
-    <row r="347" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A347" s="40">
         <v>45261</v>
       </c>
       <c r="B347" s="20"/>
-      <c r="C347" s="13"/>
+      <c r="C347" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D347" s="39"/>
       <c r="E347" s="9"/>
       <c r="F347" s="20"/>
-      <c r="G347" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G347" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H347" s="39"/>
       <c r="I347" s="9"/>
       <c r="J347" s="11"/>
       <c r="K347" s="20"/>
     </row>
-    <row r="348" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A348" s="48" t="s">
         <v>190</v>
       </c>
@@ -9203,7 +9204,7 @@
       <c r="J348" s="11"/>
       <c r="K348" s="20"/>
     </row>
-    <row r="349" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A349" s="40">
         <v>45292</v>
       </c>
@@ -9221,7 +9222,7 @@
       <c r="J349" s="11"/>
       <c r="K349" s="20"/>
     </row>
-    <row r="350" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A350" s="40">
         <v>45323</v>
       </c>
@@ -9239,7 +9240,7 @@
       <c r="J350" s="11"/>
       <c r="K350" s="20"/>
     </row>
-    <row r="351" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A351" s="40">
         <v>45352</v>
       </c>
@@ -9257,7 +9258,7 @@
       <c r="J351" s="11"/>
       <c r="K351" s="20"/>
     </row>
-    <row r="352" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A352" s="40">
         <v>45383</v>
       </c>
@@ -9275,7 +9276,7 @@
       <c r="J352" s="11"/>
       <c r="K352" s="20"/>
     </row>
-    <row r="353" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A353" s="40">
         <v>45413</v>
       </c>
@@ -9293,7 +9294,7 @@
       <c r="J353" s="11"/>
       <c r="K353" s="20"/>
     </row>
-    <row r="354" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A354" s="40">
         <v>45444</v>
       </c>
@@ -9311,7 +9312,7 @@
       <c r="J354" s="11"/>
       <c r="K354" s="20"/>
     </row>
-    <row r="355" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A355" s="40">
         <v>45474</v>
       </c>
@@ -9329,7 +9330,7 @@
       <c r="J355" s="11"/>
       <c r="K355" s="20"/>
     </row>
-    <row r="356" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A356" s="40">
         <v>45505</v>
       </c>
@@ -9347,7 +9348,7 @@
       <c r="J356" s="11"/>
       <c r="K356" s="20"/>
     </row>
-    <row r="357" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A357" s="40">
         <v>45536</v>
       </c>
@@ -9365,7 +9366,7 @@
       <c r="J357" s="11"/>
       <c r="K357" s="20"/>
     </row>
-    <row r="358" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A358" s="40">
         <v>45566</v>
       </c>
@@ -9383,7 +9384,7 @@
       <c r="J358" s="11"/>
       <c r="K358" s="20"/>
     </row>
-    <row r="359" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A359" s="40">
         <v>45597</v>
       </c>
@@ -9401,7 +9402,7 @@
       <c r="J359" s="11"/>
       <c r="K359" s="20"/>
     </row>
-    <row r="360" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A360" s="40">
         <v>45627</v>
       </c>
@@ -9419,7 +9420,7 @@
       <c r="J360" s="11"/>
       <c r="K360" s="20"/>
     </row>
-    <row r="361" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A361" s="40">
         <v>45658</v>
       </c>
@@ -9437,7 +9438,7 @@
       <c r="J361" s="11"/>
       <c r="K361" s="20"/>
     </row>
-    <row r="362" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A362" s="40">
         <v>45689</v>
       </c>
@@ -9455,7 +9456,7 @@
       <c r="J362" s="11"/>
       <c r="K362" s="20"/>
     </row>
-    <row r="363" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A363" s="40">
         <v>45717</v>
       </c>
@@ -9473,7 +9474,7 @@
       <c r="J363" s="11"/>
       <c r="K363" s="20"/>
     </row>
-    <row r="364" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A364" s="40">
         <v>45748</v>
       </c>
@@ -9491,7 +9492,7 @@
       <c r="J364" s="11"/>
       <c r="K364" s="20"/>
     </row>
-    <row r="365" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A365" s="40">
         <v>45778</v>
       </c>
@@ -9509,7 +9510,7 @@
       <c r="J365" s="11"/>
       <c r="K365" s="20"/>
     </row>
-    <row r="366" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A366" s="40">
         <v>45809</v>
       </c>
@@ -9527,7 +9528,7 @@
       <c r="J366" s="11"/>
       <c r="K366" s="20"/>
     </row>
-    <row r="367" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A367" s="40">
         <v>45839</v>
       </c>
@@ -9545,7 +9546,7 @@
       <c r="J367" s="11"/>
       <c r="K367" s="20"/>
     </row>
-    <row r="368" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A368" s="40">
         <v>45870</v>
       </c>
@@ -9563,7 +9564,7 @@
       <c r="J368" s="11"/>
       <c r="K368" s="20"/>
     </row>
-    <row r="369" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A369" s="40">
         <v>45901</v>
       </c>
@@ -9581,7 +9582,7 @@
       <c r="J369" s="11"/>
       <c r="K369" s="20"/>
     </row>
-    <row r="370" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A370" s="40">
         <v>45931</v>
       </c>
@@ -9599,7 +9600,7 @@
       <c r="J370" s="11"/>
       <c r="K370" s="20"/>
     </row>
-    <row r="371" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A371" s="40">
         <v>45962</v>
       </c>
@@ -9617,7 +9618,7 @@
       <c r="J371" s="11"/>
       <c r="K371" s="20"/>
     </row>
-    <row r="372" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A372" s="40">
         <v>45992</v>
       </c>
@@ -9635,7 +9636,7 @@
       <c r="J372" s="11"/>
       <c r="K372" s="20"/>
     </row>
-    <row r="373" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A373" s="40">
         <v>46023</v>
       </c>
@@ -9653,7 +9654,7 @@
       <c r="J373" s="11"/>
       <c r="K373" s="20"/>
     </row>
-    <row r="374" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A374" s="40">
         <v>46054</v>
       </c>
@@ -9671,7 +9672,7 @@
       <c r="J374" s="11"/>
       <c r="K374" s="20"/>
     </row>
-    <row r="375" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A375" s="40">
         <v>46082</v>
       </c>
@@ -9689,7 +9690,7 @@
       <c r="J375" s="11"/>
       <c r="K375" s="20"/>
     </row>
-    <row r="376" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A376" s="40">
         <v>46113</v>
       </c>
@@ -9707,7 +9708,7 @@
       <c r="J376" s="11"/>
       <c r="K376" s="20"/>
     </row>
-    <row r="377" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A377" s="40">
         <v>46143</v>
       </c>
@@ -9725,7 +9726,7 @@
       <c r="J377" s="11"/>
       <c r="K377" s="20"/>
     </row>
-    <row r="378" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A378" s="40">
         <v>46174</v>
       </c>
@@ -9743,7 +9744,7 @@
       <c r="J378" s="11"/>
       <c r="K378" s="20"/>
     </row>
-    <row r="379" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A379" s="40">
         <v>46204</v>
       </c>
@@ -9761,7 +9762,7 @@
       <c r="J379" s="11"/>
       <c r="K379" s="20"/>
     </row>
-    <row r="380" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A380" s="40">
         <v>46235</v>
       </c>
@@ -9779,7 +9780,7 @@
       <c r="J380" s="11"/>
       <c r="K380" s="20"/>
     </row>
-    <row r="381" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A381" s="40">
         <v>46266</v>
       </c>
@@ -9797,7 +9798,7 @@
       <c r="J381" s="11"/>
       <c r="K381" s="20"/>
     </row>
-    <row r="382" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A382" s="40">
         <v>46296</v>
       </c>
@@ -9815,7 +9816,7 @@
       <c r="J382" s="11"/>
       <c r="K382" s="20"/>
     </row>
-    <row r="383" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A383" s="40">
         <v>46327</v>
       </c>
@@ -9833,7 +9834,7 @@
       <c r="J383" s="11"/>
       <c r="K383" s="20"/>
     </row>
-    <row r="384" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A384" s="40">
         <v>46357</v>
       </c>
@@ -9851,7 +9852,7 @@
       <c r="J384" s="11"/>
       <c r="K384" s="20"/>
     </row>
-    <row r="385" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A385" s="40">
         <v>46388</v>
       </c>
@@ -9869,7 +9870,7 @@
       <c r="J385" s="11"/>
       <c r="K385" s="20"/>
     </row>
-    <row r="386" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A386" s="40"/>
       <c r="B386" s="20"/>
       <c r="C386" s="13"/>
@@ -9885,7 +9886,7 @@
       <c r="J386" s="11"/>
       <c r="K386" s="20"/>
     </row>
-    <row r="387" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A387" s="40"/>
       <c r="B387" s="20"/>
       <c r="C387" s="13"/>
@@ -9901,7 +9902,7 @@
       <c r="J387" s="11"/>
       <c r="K387" s="20"/>
     </row>
-    <row r="388" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A388" s="40"/>
       <c r="B388" s="20"/>
       <c r="C388" s="13"/>
@@ -9917,7 +9918,7 @@
       <c r="J388" s="11"/>
       <c r="K388" s="20"/>
     </row>
-    <row r="389" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A389" s="40"/>
       <c r="B389" s="20"/>
       <c r="C389" s="13"/>
@@ -9933,7 +9934,7 @@
       <c r="J389" s="11"/>
       <c r="K389" s="20"/>
     </row>
-    <row r="390" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A390" s="40"/>
       <c r="B390" s="20"/>
       <c r="C390" s="13"/>
@@ -9949,7 +9950,7 @@
       <c r="J390" s="11"/>
       <c r="K390" s="20"/>
     </row>
-    <row r="391" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A391" s="40"/>
       <c r="B391" s="20"/>
       <c r="C391" s="13"/>
@@ -9965,7 +9966,7 @@
       <c r="J391" s="11"/>
       <c r="K391" s="20"/>
     </row>
-    <row r="392" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A392" s="41"/>
       <c r="B392" s="15"/>
       <c r="C392" s="42"/>
@@ -9996,10 +9997,10 @@
     <mergeCell ref="F4:G4"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
   </dataValidations>
@@ -10022,34 +10023,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3576" topLeftCell="A34" activePane="bottomLeft"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3570" topLeftCell="A22" activePane="bottomLeft"/>
       <selection activeCell="E2" sqref="E2"/>
       <selection pane="bottomLeft" activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
@@ -10070,7 +10071,7 @@
       <c r="J2" s="54"/>
       <c r="K2" s="55"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
@@ -10088,7 +10089,7 @@
       <c r="J3" s="56"/>
       <c r="K3" s="57"/>
     </row>
-    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
@@ -10108,7 +10109,7 @@
       <c r="J4" s="54"/>
       <c r="K4" s="55"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="H5" s="27" t="s">
         <v>18</v>
@@ -10116,7 +10117,7 @@
       <c r="I5" s="27"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31"/>
@@ -10129,7 +10130,7 @@
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="C7" s="52" t="s">
@@ -10146,7 +10147,7 @@
       <c r="J7" s="52"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -10181,7 +10182,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>23</v>
@@ -10205,7 +10206,7 @@
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="48" t="s">
         <v>44</v>
       </c>
@@ -10227,7 +10228,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="40">
         <v>43101</v>
       </c>
@@ -10251,7 +10252,7 @@
         <v>43131</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="40">
         <v>43221</v>
       </c>
@@ -10275,7 +10276,7 @@
         <v>43217</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="40"/>
       <c r="B13" s="20" t="s">
         <v>50</v>
@@ -10294,7 +10295,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="40">
         <v>43313</v>
       </c>
@@ -10318,7 +10319,7 @@
         <v>43319</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="40">
         <v>43435</v>
       </c>
@@ -10342,7 +10343,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="48" t="s">
         <v>45</v>
       </c>
@@ -10360,7 +10361,7 @@
       <c r="J16" s="11"/>
       <c r="K16" s="20"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="40">
         <v>43556</v>
       </c>
@@ -10384,7 +10385,7 @@
         <v>43613</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="40">
         <v>43709</v>
       </c>
@@ -10408,7 +10409,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="40">
         <v>43770</v>
       </c>
@@ -10432,7 +10433,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="48" t="s">
         <v>46</v>
       </c>
@@ -10450,7 +10451,7 @@
       <c r="J20" s="11"/>
       <c r="K20" s="20"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="40">
         <v>43831</v>
       </c>
@@ -10472,7 +10473,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="40"/>
       <c r="B22" s="20" t="s">
         <v>54</v>
@@ -10489,7 +10490,7 @@
       <c r="J22" s="11"/>
       <c r="K22" s="20"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="40">
         <v>43862</v>
       </c>
@@ -10511,7 +10512,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="48" t="s">
         <v>47</v>
       </c>
@@ -10529,7 +10530,7 @@
       <c r="J24" s="11"/>
       <c r="K24" s="20"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="40">
         <v>44348</v>
       </c>
@@ -10553,7 +10554,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="40">
         <v>44531</v>
       </c>
@@ -10575,7 +10576,7 @@
       <c r="J26" s="11"/>
       <c r="K26" s="20"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="48" t="s">
         <v>48</v>
       </c>
@@ -10593,7 +10594,7 @@
       <c r="J27" s="11"/>
       <c r="K27" s="20"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="40">
         <v>44682</v>
       </c>
@@ -10617,7 +10618,7 @@
         <v>44691</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="40">
         <v>44774</v>
       </c>
@@ -10641,7 +10642,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="40"/>
       <c r="B30" s="20" t="s">
         <v>107</v>
@@ -10663,7 +10664,7 @@
         <v>44779</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="40">
         <v>44805</v>
       </c>
@@ -10687,7 +10688,7 @@
         <v>44805</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="40">
         <v>44896</v>
       </c>
@@ -10711,7 +10712,7 @@
         <v>44918</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="48" t="s">
         <v>66</v>
       </c>
@@ -10729,7 +10730,7 @@
       <c r="J33" s="11"/>
       <c r="K33" s="20"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="40">
         <v>44958</v>
       </c>
@@ -10753,7 +10754,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="40">
         <v>45279</v>
       </c>
@@ -10777,7 +10778,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="40"/>
       <c r="B36" s="20" t="s">
         <v>50</v>
@@ -10799,7 +10800,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="40"/>
       <c r="B37" s="20"/>
       <c r="C37" s="13"/>
@@ -10815,7 +10816,7 @@
       <c r="J37" s="11"/>
       <c r="K37" s="20"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="40"/>
       <c r="B38" s="20"/>
       <c r="C38" s="13"/>
@@ -10831,7 +10832,7 @@
       <c r="J38" s="11"/>
       <c r="K38" s="20"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="40"/>
       <c r="B39" s="20"/>
       <c r="C39" s="13"/>
@@ -10847,7 +10848,7 @@
       <c r="J39" s="11"/>
       <c r="K39" s="20"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="40"/>
       <c r="B40" s="20"/>
       <c r="C40" s="13"/>
@@ -10863,7 +10864,7 @@
       <c r="J40" s="11"/>
       <c r="K40" s="20"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="41"/>
       <c r="B41" s="15"/>
       <c r="C41" s="42"/>
@@ -10879,7 +10880,7 @@
       <c r="J41" s="12"/>
       <c r="K41" s="15"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="40"/>
       <c r="B42" s="20"/>
       <c r="C42" s="13"/>
@@ -10895,7 +10896,7 @@
       <c r="J42" s="11"/>
       <c r="K42" s="20"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="40"/>
       <c r="B43" s="20"/>
       <c r="C43" s="13"/>
@@ -10911,7 +10912,7 @@
       <c r="J43" s="11"/>
       <c r="K43" s="20"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="40"/>
       <c r="B44" s="20"/>
       <c r="C44" s="13"/>
@@ -10927,7 +10928,7 @@
       <c r="J44" s="11"/>
       <c r="K44" s="20"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="40"/>
       <c r="B45" s="20"/>
       <c r="C45" s="13"/>
@@ -10943,7 +10944,7 @@
       <c r="J45" s="11"/>
       <c r="K45" s="20"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="40"/>
       <c r="B46" s="20"/>
       <c r="C46" s="13"/>
@@ -10959,7 +10960,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="20"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="40"/>
       <c r="B47" s="20"/>
       <c r="C47" s="13"/>
@@ -10975,7 +10976,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="20"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="40"/>
       <c r="B48" s="20"/>
       <c r="C48" s="13"/>
@@ -10991,7 +10992,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="20"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="40"/>
       <c r="B49" s="20"/>
       <c r="C49" s="13"/>
@@ -11007,7 +11008,7 @@
       <c r="J49" s="11"/>
       <c r="K49" s="20"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="40"/>
       <c r="B50" s="20"/>
       <c r="C50" s="13"/>
@@ -11023,7 +11024,7 @@
       <c r="J50" s="11"/>
       <c r="K50" s="20"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="40"/>
       <c r="B51" s="20"/>
       <c r="C51" s="13"/>
@@ -11039,7 +11040,7 @@
       <c r="J51" s="11"/>
       <c r="K51" s="20"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="40"/>
       <c r="B52" s="20"/>
       <c r="C52" s="13"/>
@@ -11055,7 +11056,7 @@
       <c r="J52" s="11"/>
       <c r="K52" s="20"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="40"/>
       <c r="B53" s="20"/>
       <c r="C53" s="13"/>
@@ -11071,7 +11072,7 @@
       <c r="J53" s="11"/>
       <c r="K53" s="20"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="40"/>
       <c r="B54" s="20"/>
       <c r="C54" s="13"/>
@@ -11087,7 +11088,7 @@
       <c r="J54" s="11"/>
       <c r="K54" s="20"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="40"/>
       <c r="B55" s="20"/>
       <c r="C55" s="13"/>
@@ -11103,7 +11104,7 @@
       <c r="J55" s="11"/>
       <c r="K55" s="20"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="40"/>
       <c r="B56" s="20"/>
       <c r="C56" s="13"/>
@@ -11119,7 +11120,7 @@
       <c r="J56" s="11"/>
       <c r="K56" s="20"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="40"/>
       <c r="B57" s="20"/>
       <c r="C57" s="13"/>
@@ -11135,7 +11136,7 @@
       <c r="J57" s="11"/>
       <c r="K57" s="20"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="40"/>
       <c r="B58" s="20"/>
       <c r="C58" s="13"/>
@@ -11151,7 +11152,7 @@
       <c r="J58" s="11"/>
       <c r="K58" s="20"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="41"/>
       <c r="B59" s="15"/>
       <c r="C59" s="42"/>
@@ -11169,23 +11170,23 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="J3:K3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
   </dataValidations>
@@ -11208,28 +11209,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.109375" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
-    <col min="11" max="11" width="14.88671875" style="37" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" style="37" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D1" s="60" t="s">
         <v>33</v>
       </c>
@@ -11242,7 +11243,7 @@
       <c r="K1" s="61"/>
       <c r="L1" s="61"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>24</v>
       </c>
@@ -11271,7 +11272,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>75.253</v>
       </c>
@@ -11303,17 +11304,17 @@
         <v>1.167</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="G4" s="33"/>
       <c r="J4" s="1" t="str">
         <f>IF(TEXT(J3,"D")=1,1,TEXT(J3,"D"))</f>
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C6" s="38" t="s">
         <v>28</v>
       </c>
@@ -11334,7 +11335,7 @@
       <c r="K6" s="62"/>
       <c r="L6" s="62"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C7" s="37">
         <v>1</v>
       </c>
@@ -11361,7 +11362,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C8" s="37">
         <v>2</v>
       </c>
@@ -11387,7 +11388,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C9" s="37">
         <v>3</v>
       </c>
@@ -11413,7 +11414,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C10" s="37">
         <v>4</v>
       </c>
@@ -11439,7 +11440,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C11" s="37">
         <v>5</v>
       </c>
@@ -11465,7 +11466,7 @@
         <v>0.16700000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C12" s="37">
         <v>6</v>
       </c>
@@ -11491,7 +11492,7 @@
         <v>0.20800000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C13" s="37">
         <v>7</v>
       </c>
@@ -11517,7 +11518,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C14" s="37">
         <v>8</v>
       </c>
@@ -11543,7 +11544,7 @@
         <v>0.29199999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C15" s="37">
         <v>9</v>
       </c>
@@ -11563,7 +11564,7 @@
         <v>0.33299999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C16" s="37">
         <v>10</v>
       </c>
@@ -11583,7 +11584,7 @@
         <v>0.37499999999999994</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C17" s="37">
         <v>11</v>
       </c>
@@ -11603,7 +11604,7 @@
         <v>0.41699999999999993</v>
       </c>
     </row>
-    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C18" s="37">
         <v>12</v>
       </c>
@@ -11624,7 +11625,7 @@
         <v>0.45799999999999991</v>
       </c>
     </row>
-    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C19" s="37">
         <v>13</v>
       </c>
@@ -11645,7 +11646,7 @@
         <v>0.49999999999999989</v>
       </c>
     </row>
-    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C20" s="37">
         <v>14</v>
       </c>
@@ -11666,7 +11667,7 @@
         <v>0.54199999999999993</v>
       </c>
     </row>
-    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C21" s="37">
         <v>15</v>
       </c>
@@ -11687,7 +11688,7 @@
         <v>0.58299999999999996</v>
       </c>
     </row>
-    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C22" s="37">
         <v>16</v>
       </c>
@@ -11708,7 +11709,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C23" s="37">
         <v>17</v>
       </c>
@@ -11729,7 +11730,7 @@
         <v>0.66700000000000004</v>
       </c>
     </row>
-    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C24" s="37">
         <v>18</v>
       </c>
@@ -11750,7 +11751,7 @@
         <v>0.70800000000000007</v>
       </c>
     </row>
-    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C25" s="37">
         <v>19</v>
       </c>
@@ -11771,7 +11772,7 @@
         <v>0.75000000000000011</v>
       </c>
     </row>
-    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C26" s="37">
         <v>20</v>
       </c>
@@ -11792,7 +11793,7 @@
         <v>0.79200000000000015</v>
       </c>
     </row>
-    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C27" s="37">
         <v>21</v>
       </c>
@@ -11813,7 +11814,7 @@
         <v>0.83300000000000018</v>
       </c>
     </row>
-    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C28" s="37">
         <v>22</v>
       </c>
@@ -11834,7 +11835,7 @@
         <v>0.87500000000000022</v>
       </c>
     </row>
-    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C29" s="37">
         <v>23</v>
       </c>
@@ -11855,7 +11856,7 @@
         <v>0.91700000000000026</v>
       </c>
     </row>
-    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C30" s="37">
         <v>24</v>
       </c>
@@ -11876,7 +11877,7 @@
         <v>0.9580000000000003</v>
       </c>
     </row>
-    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C31" s="37">
         <v>25</v>
       </c>
@@ -11897,7 +11898,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C32" s="37">
         <v>26</v>
       </c>
@@ -11918,7 +11919,7 @@
         <v>1.0420000000000003</v>
       </c>
     </row>
-    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C33" s="37">
         <v>27</v>
       </c>
@@ -11939,7 +11940,7 @@
         <v>1.0830000000000002</v>
       </c>
     </row>
-    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C34" s="37">
         <v>28</v>
       </c>
@@ -11960,7 +11961,7 @@
         <v>1.1250000000000002</v>
       </c>
     </row>
-    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C35" s="37">
         <v>29</v>
       </c>
@@ -11981,7 +11982,7 @@
         <v>1.1670000000000003</v>
       </c>
     </row>
-    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C36" s="37">
         <v>30</v>
       </c>
@@ -12002,7 +12003,7 @@
         <v>1.2080000000000002</v>
       </c>
     </row>
-    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C37" s="37">
         <v>31</v>
       </c>
@@ -12023,7 +12024,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C38" s="37">
         <v>32</v>
       </c>
@@ -12032,7 +12033,7 @@
       </c>
       <c r="G38"/>
     </row>
-    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C39" s="37">
         <v>33</v>
       </c>
@@ -12041,7 +12042,7 @@
       </c>
       <c r="G39"/>
     </row>
-    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C40" s="37">
         <v>34</v>
       </c>
@@ -12050,7 +12051,7 @@
       </c>
       <c r="G40"/>
     </row>
-    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C41" s="37">
         <v>35</v>
       </c>
@@ -12059,7 +12060,7 @@
       </c>
       <c r="G41"/>
     </row>
-    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C42" s="37">
         <v>36</v>
       </c>
@@ -12068,7 +12069,7 @@
       </c>
       <c r="G42"/>
     </row>
-    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C43" s="37">
         <v>37</v>
       </c>
@@ -12077,7 +12078,7 @@
       </c>
       <c r="G43"/>
     </row>
-    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C44" s="37">
         <v>38</v>
       </c>
@@ -12086,7 +12087,7 @@
       </c>
       <c r="G44"/>
     </row>
-    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C45" s="37">
         <v>39</v>
       </c>
@@ -12095,7 +12096,7 @@
       </c>
       <c r="G45"/>
     </row>
-    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C46" s="37">
         <v>40</v>
       </c>
@@ -12104,7 +12105,7 @@
       </c>
       <c r="G46"/>
     </row>
-    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C47" s="37">
         <v>41</v>
       </c>
@@ -12113,7 +12114,7 @@
       </c>
       <c r="G47"/>
     </row>
-    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C48" s="37">
         <v>42</v>
       </c>
@@ -12122,7 +12123,7 @@
       </c>
       <c r="G48"/>
     </row>
-    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C49" s="37">
         <v>43</v>
       </c>
@@ -12131,7 +12132,7 @@
       </c>
       <c r="G49"/>
     </row>
-    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C50" s="37">
         <v>44</v>
       </c>
@@ -12140,7 +12141,7 @@
       </c>
       <c r="G50"/>
     </row>
-    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C51" s="37">
         <v>45</v>
       </c>
@@ -12149,7 +12150,7 @@
       </c>
       <c r="G51"/>
     </row>
-    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C52" s="37">
         <v>46</v>
       </c>
@@ -12158,7 +12159,7 @@
       </c>
       <c r="G52"/>
     </row>
-    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C53" s="37">
         <v>47</v>
       </c>
@@ -12167,7 +12168,7 @@
       </c>
       <c r="G53"/>
     </row>
-    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C54" s="37">
         <v>48</v>
       </c>
@@ -12176,7 +12177,7 @@
       </c>
       <c r="G54"/>
     </row>
-    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C55" s="37">
         <v>49</v>
       </c>
@@ -12185,7 +12186,7 @@
       </c>
       <c r="G55"/>
     </row>
-    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C56" s="37">
         <v>50</v>
       </c>
@@ -12194,7 +12195,7 @@
       </c>
       <c r="G56"/>
     </row>
-    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C57" s="37">
         <v>51</v>
       </c>
@@ -12203,7 +12204,7 @@
       </c>
       <c r="G57"/>
     </row>
-    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C58" s="37">
         <v>52</v>
       </c>
@@ -12212,7 +12213,7 @@
       </c>
       <c r="G58"/>
     </row>
-    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C59" s="37">
         <v>53</v>
       </c>
@@ -12221,7 +12222,7 @@
       </c>
       <c r="G59"/>
     </row>
-    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C60" s="37">
         <v>54</v>
       </c>
@@ -12230,7 +12231,7 @@
       </c>
       <c r="G60"/>
     </row>
-    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C61" s="37">
         <v>55</v>
       </c>
@@ -12239,7 +12240,7 @@
       </c>
       <c r="G61"/>
     </row>
-    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C62" s="37">
         <v>56</v>
       </c>
@@ -12248,7 +12249,7 @@
       </c>
       <c r="G62"/>
     </row>
-    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C63" s="37">
         <v>57</v>
       </c>
@@ -12257,7 +12258,7 @@
       </c>
       <c r="G63"/>
     </row>
-    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C64" s="37">
         <v>58</v>
       </c>
@@ -12266,7 +12267,7 @@
       </c>
       <c r="G64"/>
     </row>
-    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C65" s="37">
         <v>59</v>
       </c>
@@ -12275,7 +12276,7 @@
       </c>
       <c r="G65"/>
     </row>
-    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C66" s="37">
         <v>60</v>
       </c>
@@ -12284,7 +12285,7 @@
       </c>
       <c r="G66"/>
     </row>
-    <row r="67" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:12" x14ac:dyDescent="0.25">
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>

</xml_diff>